<commit_message>
update data from excel
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Testing\Project\MyShopProject\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AAC8679-7389-4182-B89D-36EABD103661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C1CA0F-BFD2-4ECB-BD87-AA68DC23D661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3360" windowWidth="17280" windowHeight="8880" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="101">
   <si>
     <t>Smoke</t>
   </si>
@@ -166,12 +166,6 @@
     <t>PaymentPage</t>
   </si>
   <si>
-    <t>OrderSummary</t>
-  </si>
-  <si>
-    <t>OrderConfirmationPage</t>
-  </si>
-  <si>
     <t>EndToEndTest</t>
   </si>
   <si>
@@ -179,12 +173,6 @@
   </si>
   <si>
     <t>User should be able to order the product</t>
-  </si>
-  <si>
-    <t>AddressPageTest</t>
-  </si>
-  <si>
-    <t>addAdressTest</t>
   </si>
   <si>
     <t>Username</t>
@@ -808,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="182" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="182" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -935,7 +923,7 @@
         <v>25</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>26</v>
@@ -994,12 +982,8 @@
       <c r="A13" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>49</v>
-      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="3" t="s">
         <v>40</v>
@@ -1018,35 +1002,17 @@
       <c r="A15" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="D15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1073,18 +1039,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1100,7 +1066,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96A2D796-D9F5-4C85-875F-05DEF9DBDBF5}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="199" zoomScaleNormal="355" workbookViewId="0">
+    <sheetView zoomScale="199" zoomScaleNormal="355" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1111,21 +1077,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C2" s="6">
         <v>5</v>
@@ -1151,12 +1117,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1187,69 +1153,69 @@
   <sheetData>
     <row r="1" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="I1" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F2" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>95</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>99</v>
       </c>
       <c r="I2" s="6">
         <v>48934</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="K2" s="6">
         <v>339520993</v>
@@ -1257,34 +1223,34 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F3" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>100</v>
       </c>
       <c r="I3" s="6">
         <v>39431</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="K3" s="6">
         <v>965424580</v>
@@ -1292,34 +1258,34 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E4" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="H4" s="6" t="s">
         <v>97</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>101</v>
       </c>
       <c r="I4" s="6">
         <v>90012</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="K4" s="6">
         <v>345568321</v>
@@ -1352,82 +1318,82 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>65</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D4" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>67</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>